<commit_message>
python auto update tool
</commit_message>
<xml_diff>
--- a/Myfile.xlsx
+++ b/Myfile.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\4.PERSONAL\5.CODING\18.CAD_Tool\Update-Title-Block\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0813D3-0D1C-4F49-9453-45ACB677268A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB7D3C4-7018-47AA-B28A-D1458E63BBD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29955" yWindow="0" windowWidth="28770" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28830" yWindow="30" windowWidth="28770" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Title Block" sheetId="1" r:id="rId1"/>
@@ -95,9 +95,6 @@
     <t/>
   </si>
   <si>
-    <t>SF0</t>
-  </si>
-  <si>
     <t>Handle: 12487F</t>
   </si>
   <si>
@@ -131,9 +128,6 @@
     <t>REVISED PER EOR COMMENTS</t>
   </si>
   <si>
-    <t>SF1</t>
-  </si>
-  <si>
     <t>Handle: 125F5C</t>
   </si>
   <si>
@@ -143,9 +137,6 @@
     <t>REVISED PER CITY COMMENTS</t>
   </si>
   <si>
-    <t>SF2</t>
-  </si>
-  <si>
     <t>Handle: 12A7E6</t>
   </si>
   <si>
@@ -162,6 +153,15 @@
   </si>
   <si>
     <t>H.P.</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
   </si>
 </sst>
 </file>
@@ -590,7 +590,7 @@
   <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,46 +679,46 @@
     </row>
     <row r="2" spans="1:22" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="N2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>19</v>
@@ -733,49 +733,49 @@
         <v>19</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="T2" s="3">
         <f ca="1">TODAY()</f>
-        <v>45439</v>
+        <v>45440</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="E3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="J3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>19</v>
@@ -802,86 +802,86 @@
         <v>19</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="T3" s="3">
         <f t="shared" ref="T3:T4" ca="1" si="0">TODAY()</f>
-        <v>45439</v>
+        <v>45440</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V3" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="E4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="G4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S4" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="T4" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45439</v>
+        <v>45440</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V4" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>